<commit_message>
added standards for some missing on objectives
mostly in multiplication
</commit_message>
<xml_diff>
--- a/K5Mathlearningobjectives.xlsx
+++ b/K5Mathlearningobjectives.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="23640" windowHeight="14880"/>
+    <workbookView xWindow="-40" yWindow="620" windowWidth="24440" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Update 9_30_15" sheetId="12" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="381">
   <si>
     <t>Open Learning Objectives: K-5 math</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Subtract two 2-digit numbers, with borrowing</t>
   </si>
   <si>
-    <t>4.NBT 4 B</t>
-  </si>
-  <si>
     <t>Solve single-step word problems with addition  or subtraction with two 2-digit numbers, not knowing which operation to use</t>
   </si>
   <si>
@@ -1147,13 +1144,31 @@
   </si>
   <si>
     <t>Solve word problems involving exponents</t>
+  </si>
+  <si>
+    <t>4.NBT.4B</t>
+  </si>
+  <si>
+    <t>2.OA.1</t>
+  </si>
+  <si>
+    <t>2.NBT.5, 2.NBT.6</t>
+  </si>
+  <si>
+    <t>5.NF.4a</t>
+  </si>
+  <si>
+    <t>4.NF.4a</t>
+  </si>
+  <si>
+    <t>5.NF.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1861,7 +1876,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1896,7 +1911,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2105,28 +2120,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I328"/>
+  <dimension ref="B2:I327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="3" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I185" sqref="I185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="4" style="8" customWidth="1"/>
-    <col min="3" max="3" width="114.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="7"/>
+    <col min="3" max="3" width="114.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="23.25">
+    <row r="2" spans="2:9" ht="23">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2192,7 @@
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
     </row>
-    <row r="6" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="6" spans="2:9" outlineLevel="1">
       <c r="B6" s="5"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
@@ -2191,7 +2206,7 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
     </row>
-    <row r="7" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="7" spans="2:9" outlineLevel="1">
       <c r="B7" s="5"/>
       <c r="C7" s="17" t="s">
         <v>6</v>
@@ -2207,7 +2222,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
     </row>
-    <row r="8" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="8" spans="2:9" outlineLevel="1">
       <c r="B8" s="5"/>
       <c r="C8" s="9" t="s">
         <v>9</v>
@@ -2223,7 +2238,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="9" spans="2:9" outlineLevel="1">
       <c r="B9" s="5"/>
       <c r="C9" s="9" t="s">
         <v>12</v>
@@ -2237,7 +2252,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="10" spans="2:9" outlineLevel="1">
       <c r="B10" s="5"/>
       <c r="C10" s="9" t="s">
         <v>13</v>
@@ -2251,7 +2266,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="11" spans="2:9" outlineLevel="1">
       <c r="B11" s="5"/>
       <c r="C11" s="9" t="s">
         <v>14</v>
@@ -2265,8 +2280,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="2:9" hidden="1" outlineLevel="1"/>
-    <row r="13" spans="2:9" collapsed="1"/>
+    <row r="12" spans="2:9" outlineLevel="1"/>
     <row r="14" spans="2:9">
       <c r="B14" s="5"/>
       <c r="C14" s="20" t="s">
@@ -2279,7 +2293,7 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="15" spans="2:9" outlineLevel="1">
       <c r="B15" s="5"/>
       <c r="C15" s="18" t="s">
         <v>16</v>
@@ -2293,7 +2307,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="16" spans="2:9" outlineLevel="1">
       <c r="B16" s="5"/>
       <c r="C16" s="9" t="s">
         <v>18</v>
@@ -2307,7 +2321,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="17" spans="2:9" outlineLevel="1">
       <c r="C17" s="9" t="s">
         <v>20</v>
       </c>
@@ -2320,7 +2334,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="18" spans="2:9" outlineLevel="1">
       <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
@@ -2333,7 +2347,7 @@
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="19" spans="2:9" outlineLevel="1">
       <c r="C19" s="9" t="s">
         <v>24</v>
       </c>
@@ -2346,7 +2360,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="20" spans="2:9" outlineLevel="1">
       <c r="C20" s="19"/>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
@@ -2355,7 +2369,7 @@
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="2:9" collapsed="1">
+    <row r="21" spans="2:9">
       <c r="C21" s="19"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
@@ -2375,7 +2389,7 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="23" spans="2:9" outlineLevel="1">
       <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2402,7 @@
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="24" spans="2:9" outlineLevel="1">
       <c r="C24" s="3" t="s">
         <v>28</v>
       </c>
@@ -2401,7 +2415,7 @@
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
     </row>
-    <row r="25" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="25" spans="2:9" outlineLevel="1">
       <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
@@ -2414,7 +2428,7 @@
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="26" spans="2:9" outlineLevel="1">
       <c r="C26" s="3" t="s">
         <v>32</v>
       </c>
@@ -2427,7 +2441,7 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="27" spans="2:9" outlineLevel="1">
       <c r="B27" s="5"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
@@ -2436,7 +2450,7 @@
       <c r="H27" s="38"/>
       <c r="I27" s="38"/>
     </row>
-    <row r="28" spans="2:9" collapsed="1">
+    <row r="28" spans="2:9">
       <c r="B28" s="5"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -2457,7 +2471,7 @@
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
     </row>
-    <row r="30" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="30" spans="2:9" outlineLevel="1">
       <c r="B30" s="5"/>
       <c r="C30" s="28" t="s">
         <v>34</v>
@@ -2471,7 +2485,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="31" spans="2:9" outlineLevel="1">
       <c r="B31" s="5"/>
       <c r="C31" s="28" t="s">
         <v>36</v>
@@ -2485,7 +2499,7 @@
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="32" spans="2:9" outlineLevel="1">
       <c r="B32" s="5"/>
       <c r="C32" s="28" t="s">
         <v>37</v>
@@ -2499,7 +2513,7 @@
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
     </row>
-    <row r="33" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="33" spans="2:9" outlineLevel="1">
       <c r="B33" s="5"/>
       <c r="C33" s="28" t="s">
         <v>38</v>
@@ -2513,7 +2527,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="34" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="34" spans="2:9" outlineLevel="1">
       <c r="B34" s="5"/>
       <c r="C34" s="28" t="s">
         <v>39</v>
@@ -2527,7 +2541,7 @@
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
     </row>
-    <row r="35" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="35" spans="2:9" outlineLevel="1">
       <c r="B35" s="5"/>
       <c r="C35" s="28" t="s">
         <v>40</v>
@@ -2541,7 +2555,7 @@
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
     </row>
-    <row r="36" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="36" spans="2:9" outlineLevel="1">
       <c r="B36" s="5"/>
       <c r="C36" s="28" t="s">
         <v>41</v>
@@ -2555,7 +2569,7 @@
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
     </row>
-    <row r="37" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="37" spans="2:9" outlineLevel="1">
       <c r="B37" s="5"/>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
@@ -2564,7 +2578,7 @@
       <c r="H37" s="38"/>
       <c r="I37" s="38"/>
     </row>
-    <row r="38" spans="2:9" collapsed="1">
+    <row r="38" spans="2:9">
       <c r="B38" s="5"/>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
@@ -2597,7 +2611,7 @@
       <c r="H40" s="38"/>
       <c r="I40" s="38"/>
     </row>
-    <row r="41" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="41" spans="2:9" outlineLevel="1">
       <c r="B41" s="5"/>
       <c r="C41" s="9" t="s">
         <v>44</v>
@@ -2611,7 +2625,7 @@
       <c r="H41" s="21"/>
       <c r="I41" s="21"/>
     </row>
-    <row r="42" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="42" spans="2:9" outlineLevel="1">
       <c r="B42" s="5"/>
       <c r="C42" s="9" t="s">
         <v>46</v>
@@ -2627,31 +2641,35 @@
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
     </row>
-    <row r="43" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="43" spans="2:9" outlineLevel="1">
       <c r="B43" s="5"/>
       <c r="C43" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
+      <c r="F43" s="21" t="s">
+        <v>376</v>
+      </c>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21"/>
     </row>
-    <row r="44" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="44" spans="2:9" outlineLevel="1">
       <c r="B44" s="5"/>
       <c r="C44" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
+      <c r="F44" s="21" t="s">
+        <v>69</v>
+      </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
     </row>
-    <row r="45" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="45" spans="2:9" outlineLevel="1">
       <c r="B45" s="5"/>
       <c r="C45" s="9" t="s">
         <v>51</v>
@@ -2659,13 +2677,13 @@
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
       <c r="F45" s="21" t="s">
-        <v>52</v>
+        <v>377</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
     </row>
-    <row r="46" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="46" spans="2:9" outlineLevel="1">
       <c r="B46" s="5"/>
       <c r="C46" s="9" t="s">
         <v>53</v>
@@ -2679,7 +2697,7 @@
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
     </row>
-    <row r="47" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="47" spans="2:9" outlineLevel="1">
       <c r="B47" s="5"/>
       <c r="C47" s="9" t="s">
         <v>54</v>
@@ -2693,19 +2711,21 @@
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
     </row>
-    <row r="48" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="48" spans="2:9" outlineLevel="1">
       <c r="B48" s="5"/>
       <c r="C48" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+      <c r="F48" s="21" t="s">
+        <v>376</v>
+      </c>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
     </row>
-    <row r="49" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="49" spans="2:9" outlineLevel="1">
       <c r="B49" s="5"/>
       <c r="C49" s="9" t="s">
         <v>57</v>
@@ -2721,7 +2741,7 @@
       </c>
       <c r="I49" s="21"/>
     </row>
-    <row r="50" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="50" spans="2:9" outlineLevel="1">
       <c r="B50" s="5"/>
       <c r="C50" s="9" t="s">
         <v>60</v>
@@ -2737,7 +2757,7 @@
       </c>
       <c r="I50" s="21"/>
     </row>
-    <row r="51" spans="2:9" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="51" spans="2:9" outlineLevel="1" collapsed="1">
       <c r="B51" s="5"/>
       <c r="D51" s="38"/>
       <c r="E51" s="38"/>
@@ -2746,7 +2766,7 @@
       <c r="H51" s="38"/>
       <c r="I51" s="38"/>
     </row>
-    <row r="52" spans="2:9" collapsed="1">
+    <row r="52" spans="2:9">
       <c r="B52" s="5"/>
       <c r="C52" s="20" t="s">
         <v>62</v>
@@ -2758,7 +2778,7 @@
       <c r="H52" s="38"/>
       <c r="I52" s="38"/>
     </row>
-    <row r="53" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="53" spans="2:9" outlineLevel="1">
       <c r="B53" s="5"/>
       <c r="C53" s="9" t="s">
         <v>63</v>
@@ -2772,7 +2792,7 @@
       <c r="H53" s="21"/>
       <c r="I53" s="21"/>
     </row>
-    <row r="54" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="54" spans="2:9" outlineLevel="1">
       <c r="B54" s="5"/>
       <c r="C54" s="9" t="s">
         <v>65</v>
@@ -2786,7 +2806,7 @@
       <c r="H54" s="21"/>
       <c r="I54" s="21"/>
     </row>
-    <row r="55" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="55" spans="2:9" outlineLevel="1">
       <c r="B55" s="5"/>
       <c r="C55" s="9" t="s">
         <v>66</v>
@@ -2800,7 +2820,7 @@
       <c r="H55" s="21"/>
       <c r="I55" s="21"/>
     </row>
-    <row r="56" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="56" spans="2:9" outlineLevel="1">
       <c r="B56" s="5"/>
       <c r="C56" s="9" t="s">
         <v>67</v>
@@ -2812,7 +2832,7 @@
       <c r="H56" s="21"/>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="57" spans="2:9" outlineLevel="1">
       <c r="B57" s="5"/>
       <c r="C57" s="9" t="s">
         <v>68</v>
@@ -2826,7 +2846,7 @@
       <c r="H57" s="21"/>
       <c r="I57" s="21"/>
     </row>
-    <row r="58" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="58" spans="2:9" outlineLevel="1">
       <c r="B58" s="5"/>
       <c r="C58" s="9" t="s">
         <v>70</v>
@@ -2838,14 +2858,14 @@
       </c>
       <c r="G58" s="21"/>
       <c r="H58" s="21" t="s">
-        <v>71</v>
+        <v>375</v>
       </c>
       <c r="I58" s="21"/>
     </row>
-    <row r="59" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="59" spans="2:9" outlineLevel="1">
       <c r="B59" s="5"/>
       <c r="C59" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
@@ -2856,10 +2876,10 @@
       <c r="H59" s="21"/>
       <c r="I59" s="21"/>
     </row>
-    <row r="60" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="60" spans="2:9" outlineLevel="1">
       <c r="B60" s="5"/>
       <c r="C60" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
@@ -2870,10 +2890,10 @@
       <c r="H60" s="21"/>
       <c r="I60" s="21"/>
     </row>
-    <row r="61" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="61" spans="2:9" outlineLevel="1">
       <c r="B61" s="5"/>
       <c r="C61" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
@@ -2884,7 +2904,7 @@
       <c r="H61" s="21"/>
       <c r="I61" s="21"/>
     </row>
-    <row r="62" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="62" spans="2:9" outlineLevel="1">
       <c r="B62" s="5"/>
       <c r="C62" s="22"/>
       <c r="D62" s="38"/>
@@ -2894,10 +2914,10 @@
       <c r="H62" s="38"/>
       <c r="I62" s="38"/>
     </row>
-    <row r="63" spans="2:9" collapsed="1">
+    <row r="63" spans="2:9">
       <c r="B63" s="5"/>
       <c r="C63" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D63" s="38"/>
       <c r="E63" s="38"/>
@@ -2906,24 +2926,24 @@
       <c r="H63" s="38"/>
       <c r="I63" s="38"/>
     </row>
-    <row r="64" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="64" spans="2:9" outlineLevel="1">
       <c r="B64" s="5"/>
       <c r="C64" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
       <c r="F64" s="21"/>
       <c r="G64" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H64" s="21"/>
       <c r="I64" s="21"/>
     </row>
-    <row r="65" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="65" spans="2:9" outlineLevel="1">
       <c r="B65" s="5"/>
       <c r="C65" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
@@ -2931,81 +2951,83 @@
       <c r="G65" s="21"/>
       <c r="H65" s="21"/>
       <c r="I65" s="21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" hidden="1" outlineLevel="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" outlineLevel="1">
       <c r="B66" s="5"/>
       <c r="C66" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21"/>
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
+      <c r="H66" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="I66" s="21"/>
     </row>
-    <row r="67" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="67" spans="2:9" outlineLevel="1">
       <c r="B67" s="5"/>
       <c r="C67" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
       <c r="F67" s="21"/>
       <c r="G67" s="21"/>
       <c r="H67" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I67" s="21"/>
     </row>
-    <row r="68" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="68" spans="2:9" outlineLevel="1">
       <c r="B68" s="5"/>
       <c r="C68" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="21"/>
       <c r="G68" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H68" s="21"/>
       <c r="I68" s="21"/>
     </row>
-    <row r="69" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="69" spans="2:9" outlineLevel="1">
       <c r="B69" s="5"/>
       <c r="C69" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
       <c r="G69" s="21"/>
       <c r="H69" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I69" s="21"/>
     </row>
-    <row r="70" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="70" spans="2:9" outlineLevel="1">
       <c r="B70" s="5"/>
       <c r="C70" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
       <c r="F70" s="21"/>
       <c r="G70" s="21"/>
       <c r="H70" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I70" s="21"/>
     </row>
-    <row r="71" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="71" spans="2:9" outlineLevel="1">
       <c r="B71" s="5"/>
       <c r="C71" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
@@ -3014,16 +3036,16 @@
       <c r="H71" s="21"/>
       <c r="I71" s="21"/>
     </row>
-    <row r="72" spans="2:9" hidden="1" outlineLevel="1"/>
-    <row r="73" spans="2:9" collapsed="1">
+    <row r="72" spans="2:9" outlineLevel="1"/>
+    <row r="73" spans="2:9">
       <c r="C73" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" hidden="1" outlineLevel="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" outlineLevel="1">
       <c r="B74" s="5"/>
       <c r="C74" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
@@ -3031,13 +3053,13 @@
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
       <c r="I74" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" hidden="1" outlineLevel="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" outlineLevel="1">
       <c r="B75" s="5"/>
       <c r="C75" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
@@ -3045,69 +3067,69 @@
       <c r="G75" s="21"/>
       <c r="H75" s="21"/>
       <c r="I75" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" hidden="1" outlineLevel="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" outlineLevel="1">
       <c r="B76" s="5"/>
       <c r="C76" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
       <c r="F76" s="21"/>
       <c r="G76" s="21"/>
       <c r="H76" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I76" s="21"/>
     </row>
-    <row r="77" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="77" spans="2:9" outlineLevel="1">
       <c r="B77" s="5"/>
       <c r="C77" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
       <c r="F77" s="21"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I77" s="21"/>
     </row>
-    <row r="78" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="78" spans="2:9" outlineLevel="1">
       <c r="B78" s="5"/>
       <c r="C78" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
       <c r="F78" s="21"/>
       <c r="G78" s="21"/>
       <c r="H78" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I78" s="21"/>
     </row>
-    <row r="79" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="79" spans="2:9" outlineLevel="1">
       <c r="B79" s="5"/>
       <c r="C79" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
       <c r="G79" s="21"/>
       <c r="H79" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I79" s="21"/>
     </row>
-    <row r="80" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="80" spans="2:9" outlineLevel="1">
       <c r="B80" s="5"/>
       <c r="C80" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
@@ -3115,115 +3137,115 @@
       <c r="G80" s="21"/>
       <c r="H80" s="21"/>
       <c r="I80" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" hidden="1" outlineLevel="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" outlineLevel="1">
       <c r="B81" s="5"/>
       <c r="C81" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
       <c r="F81" s="21"/>
       <c r="G81" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H81" s="21"/>
       <c r="I81" s="21"/>
     </row>
-    <row r="82" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="82" spans="2:9" outlineLevel="1">
       <c r="B82" s="5"/>
       <c r="C82" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
       <c r="F82" s="21"/>
       <c r="G82" s="21"/>
       <c r="H82" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I82" s="21"/>
     </row>
-    <row r="83" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="83" spans="2:9" outlineLevel="1">
       <c r="B83" s="5"/>
       <c r="C83" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
       <c r="H83" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I83" s="21"/>
     </row>
-    <row r="84" spans="2:9" hidden="1" outlineLevel="1"/>
-    <row r="85" spans="2:9" collapsed="1">
+    <row r="84" spans="2:9" outlineLevel="1"/>
+    <row r="85" spans="2:9">
       <c r="C85" s="5"/>
     </row>
     <row r="86" spans="2:9">
       <c r="C86" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" outlineLevel="1">
+      <c r="C87" s="15" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="87" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C87" s="15" t="s">
-        <v>104</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
       <c r="G87" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H87" s="21"/>
       <c r="I87" s="21"/>
     </row>
-    <row r="88" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="88" spans="2:9" outlineLevel="1">
       <c r="C88" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
       <c r="G88" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H88" s="21"/>
       <c r="I88" s="21"/>
     </row>
-    <row r="89" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="89" spans="2:9" outlineLevel="1">
       <c r="C89" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
       <c r="F89" s="21"/>
       <c r="G89" s="21"/>
       <c r="H89" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I89" s="21"/>
+    </row>
+    <row r="90" spans="2:9" outlineLevel="1">
+      <c r="C90" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="I89" s="21"/>
-    </row>
-    <row r="90" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C90" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
       <c r="F90" s="21"/>
       <c r="G90" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H90" s="21"/>
       <c r="I90" s="21"/>
     </row>
-    <row r="91" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="91" spans="2:9" outlineLevel="1">
       <c r="C91" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
@@ -3231,67 +3253,68 @@
       <c r="G91" s="21"/>
       <c r="H91" s="21"/>
       <c r="I91" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" outlineLevel="1">
+      <c r="C92" s="15" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C92" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
       <c r="H92" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I92" s="21"/>
     </row>
-    <row r="93" spans="2:9" hidden="1" outlineLevel="1"/>
-    <row r="94" spans="2:9" collapsed="1"/>
+    <row r="93" spans="2:9" outlineLevel="1"/>
     <row r="95" spans="2:9">
       <c r="C95" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" outlineLevel="1">
+      <c r="C96" s="12" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C96" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
       <c r="F96" s="21"/>
       <c r="G96" s="21"/>
       <c r="H96" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="I96" s="21"/>
+    </row>
+    <row r="97" spans="2:9" outlineLevel="1">
+      <c r="C97" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="I96" s="21"/>
-    </row>
-    <row r="97" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C97" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="D97" s="21"/>
       <c r="E97" s="21"/>
       <c r="F97" s="21"/>
       <c r="G97" s="21"/>
       <c r="H97" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I97" s="21"/>
     </row>
-    <row r="98" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="98" spans="2:9" outlineLevel="1">
       <c r="C98" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D98" s="21"/>
       <c r="E98" s="21"/>
       <c r="F98" s="21"/>
-      <c r="G98" s="21"/>
+      <c r="G98" s="21" t="s">
+        <v>139</v>
+      </c>
       <c r="H98" s="21"/>
       <c r="I98" s="21"/>
     </row>
-    <row r="99" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="99" spans="2:9" outlineLevel="1">
       <c r="D99" s="38"/>
       <c r="E99" s="38"/>
       <c r="F99" s="38"/>
@@ -3299,7 +3322,7 @@
       <c r="H99" s="38"/>
       <c r="I99" s="38"/>
     </row>
-    <row r="100" spans="2:9" collapsed="1">
+    <row r="100" spans="2:9">
       <c r="D100" s="38"/>
       <c r="E100" s="38"/>
       <c r="F100" s="38"/>
@@ -3309,50 +3332,50 @@
     </row>
     <row r="101" spans="2:9">
       <c r="C101" s="20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="2:9" hidden="1" outlineLevel="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" outlineLevel="1">
       <c r="B102" s="5"/>
       <c r="C102" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D102" s="21"/>
       <c r="E102" s="21"/>
       <c r="F102" s="21"/>
       <c r="G102" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H102" s="21"/>
       <c r="I102" s="21"/>
     </row>
-    <row r="103" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="103" spans="2:9" outlineLevel="1">
       <c r="C103" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D103" s="21"/>
       <c r="E103" s="21"/>
       <c r="F103" s="21"/>
       <c r="G103" s="21"/>
       <c r="H103" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="I103" s="21"/>
+    </row>
+    <row r="104" spans="2:9" outlineLevel="1">
+      <c r="C104" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="I103" s="21"/>
-    </row>
-    <row r="104" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C104" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
       <c r="F104" s="21"/>
       <c r="G104" s="21"/>
       <c r="H104" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I104" s="21"/>
     </row>
-    <row r="105" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="105" spans="2:9" outlineLevel="1">
       <c r="B105" s="5"/>
       <c r="C105" s="24"/>
       <c r="D105" s="38"/>
@@ -3362,7 +3385,7 @@
       <c r="H105" s="38"/>
       <c r="I105" s="38"/>
     </row>
-    <row r="106" spans="2:9" collapsed="1">
+    <row r="106" spans="2:9">
       <c r="B106" s="5"/>
       <c r="C106" s="24"/>
       <c r="D106" s="38"/>
@@ -3374,420 +3397,418 @@
     </row>
     <row r="107" spans="2:9">
       <c r="C107" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" outlineLevel="1">
+      <c r="C108" s="3" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="108" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C108" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
       <c r="F108" s="21"/>
       <c r="G108" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H108" s="21"/>
       <c r="I108" s="21"/>
     </row>
-    <row r="109" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="109" spans="2:9" outlineLevel="1">
       <c r="C109" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
       <c r="F109" s="21"/>
       <c r="G109" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H109" s="21"/>
       <c r="I109" s="21"/>
     </row>
-    <row r="110" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="110" spans="2:9" outlineLevel="1">
       <c r="C110" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
       <c r="F110" s="21"/>
       <c r="G110" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H110" s="21"/>
       <c r="I110" s="21"/>
     </row>
-    <row r="111" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="111" spans="2:9" outlineLevel="1">
       <c r="C111" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
       <c r="F111" s="21"/>
       <c r="G111" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H111" s="21"/>
       <c r="I111" s="21"/>
     </row>
-    <row r="112" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="112" spans="2:9" outlineLevel="1">
       <c r="C112" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D112" s="21"/>
       <c r="E112" s="21"/>
       <c r="F112" s="21"/>
       <c r="G112" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H112" s="21"/>
       <c r="I112" s="21"/>
     </row>
-    <row r="113" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="113" spans="3:9" outlineLevel="1">
       <c r="C113" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D113" s="21"/>
       <c r="E113" s="21"/>
       <c r="F113" s="21"/>
       <c r="G113" s="21"/>
       <c r="H113" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="I113" s="21"/>
+    </row>
+    <row r="114" spans="3:9" outlineLevel="1">
+      <c r="C114" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="I113" s="21"/>
-    </row>
-    <row r="114" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C114" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="D114" s="21"/>
       <c r="E114" s="21"/>
       <c r="F114" s="21"/>
       <c r="G114" s="21"/>
       <c r="H114" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I114" s="21"/>
     </row>
-    <row r="115" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="116" spans="3:9" collapsed="1"/>
+    <row r="115" spans="3:9" outlineLevel="1"/>
     <row r="117" spans="3:9">
       <c r="C117" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="3:9">
       <c r="C118" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" outlineLevel="1">
+      <c r="C119" s="3" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="119" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C119" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D119" s="21"/>
       <c r="E119" s="21"/>
       <c r="F119" s="21"/>
       <c r="G119" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H119" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H119" s="21" t="s">
+      <c r="I119" s="21"/>
+    </row>
+    <row r="120" spans="3:9" outlineLevel="1">
+      <c r="C120" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="I119" s="21"/>
-    </row>
-    <row r="120" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C120" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21"/>
       <c r="F120" s="21"/>
       <c r="G120" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H120" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H120" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I120" s="21"/>
     </row>
-    <row r="121" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="121" spans="3:9" outlineLevel="1">
       <c r="C121" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D121" s="21"/>
       <c r="E121" s="21"/>
       <c r="F121" s="21"/>
       <c r="G121" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H121" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H121" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I121" s="21"/>
     </row>
-    <row r="122" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="122" spans="3:9" outlineLevel="1">
       <c r="C122" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D122" s="21"/>
       <c r="E122" s="21"/>
       <c r="F122" s="21"/>
       <c r="G122" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H122" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H122" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I122" s="21"/>
     </row>
-    <row r="123" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="123" spans="3:9" outlineLevel="1">
       <c r="C123" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D123" s="21"/>
       <c r="E123" s="21"/>
       <c r="F123" s="21"/>
       <c r="G123" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H123" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H123" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I123" s="21"/>
     </row>
-    <row r="124" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="125" spans="3:9" collapsed="1">
+    <row r="124" spans="3:9" outlineLevel="1"/>
+    <row r="125" spans="3:9">
       <c r="C125" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="126" spans="3:9" outlineLevel="1">
+      <c r="C126" s="3" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="126" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C126" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D126" s="21"/>
       <c r="E126" s="21"/>
       <c r="F126" s="21"/>
       <c r="G126" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H126" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H126" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I126" s="21"/>
     </row>
-    <row r="127" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="127" spans="3:9" outlineLevel="1">
       <c r="C127" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D127" s="21"/>
       <c r="E127" s="21"/>
       <c r="F127" s="21"/>
       <c r="G127" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H127" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H127" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I127" s="21"/>
     </row>
-    <row r="128" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="128" spans="3:9" outlineLevel="1">
       <c r="C128" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D128" s="21"/>
       <c r="E128" s="21"/>
       <c r="F128" s="21"/>
       <c r="G128" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H128" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H128" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I128" s="21"/>
     </row>
-    <row r="129" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="129" spans="3:9" outlineLevel="1">
       <c r="C129" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D129" s="21"/>
       <c r="E129" s="21"/>
       <c r="F129" s="21"/>
       <c r="G129" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H129" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H129" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I129" s="21"/>
     </row>
-    <row r="130" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="130" spans="3:9" outlineLevel="1">
       <c r="C130" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D130" s="21"/>
       <c r="E130" s="21"/>
       <c r="F130" s="21"/>
       <c r="G130" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H130" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H130" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I130" s="21"/>
     </row>
-    <row r="131" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="132" spans="3:9" collapsed="1">
+    <row r="131" spans="3:9" outlineLevel="1"/>
+    <row r="132" spans="3:9">
       <c r="C132" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" outlineLevel="1">
+      <c r="C133" s="3" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="133" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C133" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D133" s="21"/>
       <c r="E133" s="21"/>
       <c r="F133" s="21"/>
       <c r="G133" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H133" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H133" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I133" s="21"/>
     </row>
-    <row r="134" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="134" spans="3:9" outlineLevel="1">
       <c r="C134" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D134" s="21"/>
       <c r="E134" s="21"/>
       <c r="F134" s="21"/>
       <c r="G134" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H134" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H134" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I134" s="21"/>
     </row>
-    <row r="135" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="135" spans="3:9" outlineLevel="1">
       <c r="C135" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D135" s="21"/>
       <c r="E135" s="21"/>
       <c r="F135" s="21"/>
       <c r="G135" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H135" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H135" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I135" s="21"/>
     </row>
-    <row r="136" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="136" spans="3:9" outlineLevel="1">
       <c r="C136" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D136" s="21"/>
       <c r="E136" s="21"/>
       <c r="F136" s="21"/>
       <c r="G136" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H136" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H136" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I136" s="21"/>
     </row>
-    <row r="137" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="138" spans="3:9" collapsed="1">
+    <row r="137" spans="3:9" outlineLevel="1"/>
+    <row r="138" spans="3:9">
       <c r="C138" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="139" spans="3:9" outlineLevel="1">
+      <c r="C139" s="3" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="139" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C139" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="D139" s="21"/>
       <c r="E139" s="21"/>
       <c r="F139" s="21"/>
       <c r="G139" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H139" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H139" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I139" s="21"/>
     </row>
-    <row r="140" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="140" spans="3:9" outlineLevel="1">
       <c r="C140" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D140" s="21"/>
       <c r="E140" s="21"/>
       <c r="F140" s="21"/>
       <c r="G140" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H140" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H140" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I140" s="21"/>
     </row>
-    <row r="141" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="141" spans="3:9" outlineLevel="1">
       <c r="C141" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D141" s="21"/>
       <c r="E141" s="21"/>
       <c r="F141" s="21"/>
       <c r="G141" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H141" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H141" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I141" s="21"/>
     </row>
-    <row r="142" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="142" spans="3:9" outlineLevel="1">
       <c r="C142" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="21"/>
       <c r="F142" s="21"/>
       <c r="G142" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H142" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H142" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I142" s="21"/>
     </row>
-    <row r="143" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="143" spans="3:9" outlineLevel="1">
       <c r="C143" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="21"/>
       <c r="G143" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H143" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="H143" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="I143" s="21"/>
     </row>
-    <row r="144" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="145" spans="2:9" collapsed="1"/>
+    <row r="144" spans="3:9" outlineLevel="1"/>
     <row r="146" spans="2:9">
       <c r="C146" s="35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D146" s="38"/>
       <c r="E146" s="38"/>
@@ -3796,22 +3817,22 @@
       <c r="H146" s="38"/>
       <c r="I146" s="38"/>
     </row>
-    <row r="147" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="147" spans="2:9" outlineLevel="1">
       <c r="C147" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D147" s="21"/>
       <c r="E147" s="21"/>
       <c r="F147" s="21"/>
       <c r="G147" s="21"/>
       <c r="H147" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I147" s="21"/>
     </row>
-    <row r="148" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="148" spans="2:9" outlineLevel="1">
       <c r="C148" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D148" s="21"/>
       <c r="E148" s="21"/>
@@ -3822,91 +3843,91 @@
       <c r="H148" s="21"/>
       <c r="I148" s="21"/>
     </row>
-    <row r="149" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="149" spans="2:9" outlineLevel="1">
       <c r="C149" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D149" s="21"/>
       <c r="E149" s="21"/>
       <c r="F149" s="21"/>
       <c r="G149" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="H149" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="H149" s="21" t="s">
+      <c r="I149" s="21"/>
+    </row>
+    <row r="150" spans="2:9" outlineLevel="1">
+      <c r="C150" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="I149" s="21"/>
-    </row>
-    <row r="150" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C150" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="D150" s="21"/>
       <c r="E150" s="21"/>
       <c r="F150" s="21"/>
       <c r="G150" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H150" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="I150" s="21"/>
+    </row>
+    <row r="151" spans="2:9" outlineLevel="1">
+      <c r="C151" s="15" t="s">
         <v>170</v>
-      </c>
-      <c r="I150" s="21"/>
-    </row>
-    <row r="151" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C151" s="15" t="s">
-        <v>171</v>
       </c>
       <c r="D151" s="21"/>
       <c r="E151" s="21"/>
       <c r="F151" s="21"/>
       <c r="G151" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H151" s="21"/>
       <c r="I151" s="21"/>
     </row>
-    <row r="152" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="152" spans="2:9" outlineLevel="1">
       <c r="C152" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="21"/>
       <c r="G152" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H152" s="21"/>
       <c r="I152" s="21"/>
     </row>
-    <row r="153" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="153" spans="2:9" outlineLevel="1">
       <c r="C153" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D153" s="21"/>
       <c r="E153" s="21"/>
       <c r="F153" s="21"/>
       <c r="G153" s="21"/>
       <c r="H153" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="I153" s="21"/>
+    </row>
+    <row r="154" spans="2:9" ht="28" outlineLevel="1">
+      <c r="C154" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="I153" s="21"/>
-    </row>
-    <row r="154" spans="2:9" ht="30" hidden="1" outlineLevel="1">
-      <c r="C154" s="23" t="s">
-        <v>176</v>
       </c>
       <c r="D154" s="21"/>
       <c r="E154" s="21"/>
       <c r="F154" s="21"/>
       <c r="G154" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H154" s="21"/>
       <c r="I154" s="21"/>
     </row>
-    <row r="155" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="155" spans="2:9" outlineLevel="1">
       <c r="C155" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D155" s="21"/>
       <c r="E155" s="21"/>
@@ -3914,10 +3935,10 @@
       <c r="G155" s="21"/>
       <c r="H155" s="21"/>
       <c r="I155" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="156" spans="2:9" hidden="1" outlineLevel="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="156" spans="2:9" outlineLevel="1">
       <c r="B156" s="7"/>
       <c r="D156" s="38"/>
       <c r="E156" s="38"/>
@@ -3926,9 +3947,9 @@
       <c r="H156" s="38"/>
       <c r="I156" s="38"/>
     </row>
-    <row r="157" spans="2:9" collapsed="1">
+    <row r="157" spans="2:9">
       <c r="C157" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D157" s="38"/>
       <c r="E157" s="38"/>
@@ -3937,124 +3958,124 @@
       <c r="H157" s="38"/>
       <c r="I157" s="38"/>
     </row>
-    <row r="158" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="158" spans="2:9" outlineLevel="1">
       <c r="C158" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D158" s="21"/>
       <c r="E158" s="21"/>
       <c r="F158" s="21"/>
       <c r="G158" s="21"/>
       <c r="H158" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="I158" s="21"/>
+    </row>
+    <row r="159" spans="2:9" outlineLevel="1">
+      <c r="C159" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="I158" s="21"/>
-    </row>
-    <row r="159" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C159" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="D159" s="21"/>
       <c r="E159" s="21"/>
       <c r="F159" s="21"/>
       <c r="G159" s="21"/>
       <c r="H159" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I159" s="21"/>
     </row>
-    <row r="160" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="160" spans="2:9" outlineLevel="1">
       <c r="C160" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D160" s="21"/>
       <c r="E160" s="21"/>
       <c r="F160" s="21"/>
       <c r="G160" s="21"/>
       <c r="H160" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="I160" s="21"/>
+    </row>
+    <row r="161" spans="3:9" outlineLevel="1">
+      <c r="C161" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="I160" s="21"/>
-    </row>
-    <row r="161" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C161" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="D161" s="21"/>
       <c r="E161" s="21"/>
       <c r="F161" s="21"/>
       <c r="G161" s="21"/>
       <c r="H161" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I161" s="21"/>
     </row>
-    <row r="162" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="162" spans="3:9" outlineLevel="1">
       <c r="C162" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D162" s="21"/>
       <c r="E162" s="21"/>
       <c r="F162" s="21"/>
       <c r="G162" s="21"/>
       <c r="H162" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="I162" s="21"/>
+    </row>
+    <row r="163" spans="3:9" outlineLevel="1">
+      <c r="C163" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="I162" s="21"/>
-    </row>
-    <row r="163" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C163" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="D163" s="21"/>
       <c r="E163" s="21"/>
       <c r="F163" s="21"/>
       <c r="G163" s="21"/>
       <c r="H163" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I163" s="21"/>
     </row>
-    <row r="164" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="164" spans="3:9" outlineLevel="1">
       <c r="C164" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D164" s="21"/>
       <c r="E164" s="21"/>
       <c r="F164" s="21"/>
       <c r="G164" s="21"/>
       <c r="H164" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="I164" s="21"/>
+    </row>
+    <row r="165" spans="3:9" outlineLevel="1">
+      <c r="C165" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="I164" s="21"/>
-    </row>
-    <row r="165" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C165" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="D165" s="21"/>
       <c r="E165" s="21"/>
       <c r="F165" s="21"/>
       <c r="G165" s="21"/>
       <c r="H165" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I165" s="21"/>
     </row>
-    <row r="166" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="166" spans="3:9" outlineLevel="1">
       <c r="C166" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D166" s="21"/>
       <c r="E166" s="21"/>
       <c r="F166" s="21"/>
       <c r="G166" s="21"/>
       <c r="H166" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I166" s="21"/>
     </row>
-    <row r="167" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="167" spans="3:9" outlineLevel="1">
       <c r="D167" s="38"/>
       <c r="E167" s="38"/>
       <c r="F167" s="38"/>
@@ -4062,9 +4083,9 @@
       <c r="H167" s="38"/>
       <c r="I167" s="38"/>
     </row>
-    <row r="168" spans="3:9" collapsed="1">
+    <row r="168" spans="3:9">
       <c r="C168" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D168" s="38"/>
       <c r="E168" s="38"/>
@@ -4073,87 +4094,87 @@
       <c r="H168" s="38"/>
       <c r="I168" s="38"/>
     </row>
-    <row r="169" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="169" spans="3:9" outlineLevel="1">
       <c r="C169" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D169" s="21"/>
       <c r="E169" s="21"/>
       <c r="F169" s="21"/>
       <c r="G169" s="21"/>
       <c r="H169" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="I169" s="21"/>
+    </row>
+    <row r="170" spans="3:9" outlineLevel="1">
+      <c r="C170" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="I169" s="21"/>
-    </row>
-    <row r="170" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C170" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="D170" s="21"/>
       <c r="E170" s="21"/>
       <c r="F170" s="21"/>
       <c r="G170" s="21"/>
       <c r="H170" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I170" s="21"/>
     </row>
-    <row r="171" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="171" spans="3:9" outlineLevel="1">
       <c r="C171" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D171" s="21"/>
       <c r="E171" s="21"/>
       <c r="F171" s="21"/>
       <c r="G171" s="21"/>
       <c r="H171" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I171" s="21"/>
     </row>
-    <row r="172" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="172" spans="3:9" outlineLevel="1">
       <c r="C172" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D172" s="21"/>
       <c r="E172" s="21"/>
       <c r="F172" s="21"/>
       <c r="G172" s="21"/>
       <c r="H172" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I172" s="21"/>
     </row>
-    <row r="173" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="173" spans="3:9" outlineLevel="1">
       <c r="C173" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D173" s="21"/>
       <c r="E173" s="21"/>
       <c r="F173" s="21"/>
       <c r="G173" s="21"/>
       <c r="H173" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I173" s="21"/>
     </row>
-    <row r="174" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="174" spans="3:9" outlineLevel="1">
       <c r="C174" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
       <c r="F174" s="21"/>
       <c r="G174" s="21"/>
       <c r="H174" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="I174" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="I174" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="175" spans="3:9" hidden="1" outlineLevel="1">
+    </row>
+    <row r="175" spans="3:9" outlineLevel="1">
       <c r="D175" s="38"/>
       <c r="E175" s="38"/>
       <c r="F175" s="38"/>
@@ -4161,9 +4182,9 @@
       <c r="H175" s="38"/>
       <c r="I175" s="38"/>
     </row>
-    <row r="176" spans="3:9" collapsed="1">
+    <row r="176" spans="3:9">
       <c r="C176" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D176" s="38"/>
       <c r="E176" s="38"/>
@@ -4172,42 +4193,48 @@
       <c r="H176" s="38"/>
       <c r="I176" s="38"/>
     </row>
-    <row r="177" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="177" spans="3:9" outlineLevel="1">
       <c r="C177" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D177" s="21"/>
       <c r="E177" s="21"/>
       <c r="F177" s="21"/>
       <c r="G177" s="21"/>
-      <c r="H177" s="21"/>
+      <c r="H177" s="21" t="s">
+        <v>213</v>
+      </c>
       <c r="I177" s="21"/>
     </row>
-    <row r="178" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="178" spans="3:9" outlineLevel="1">
       <c r="C178" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D178" s="21"/>
       <c r="E178" s="21"/>
       <c r="F178" s="21"/>
       <c r="G178" s="21"/>
       <c r="H178" s="21"/>
-      <c r="I178" s="21"/>
-    </row>
-    <row r="179" spans="3:9" hidden="1" outlineLevel="1">
+      <c r="I178" s="21" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="179" spans="3:9" outlineLevel="1">
       <c r="C179" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D179" s="21"/>
       <c r="E179" s="21"/>
       <c r="F179" s="21"/>
       <c r="G179" s="21"/>
-      <c r="H179" s="21"/>
+      <c r="H179" s="21" t="s">
+        <v>379</v>
+      </c>
       <c r="I179" s="21"/>
     </row>
-    <row r="180" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="180" spans="3:9" outlineLevel="1">
       <c r="C180" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D180" s="21"/>
       <c r="E180" s="21"/>
@@ -4215,56 +4242,62 @@
       <c r="G180" s="21"/>
       <c r="H180" s="21"/>
       <c r="I180" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="181" spans="3:9" outlineLevel="1">
+      <c r="C181" s="33" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="181" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C181" s="33" t="s">
-        <v>211</v>
       </c>
       <c r="D181" s="21"/>
       <c r="E181" s="21"/>
       <c r="F181" s="21"/>
       <c r="G181" s="21"/>
       <c r="H181" s="21"/>
-      <c r="I181" s="21"/>
-    </row>
-    <row r="182" spans="3:9" hidden="1" outlineLevel="1">
+      <c r="I181" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="182" spans="3:9" outlineLevel="1">
       <c r="C182" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D182" s="21"/>
       <c r="E182" s="21"/>
       <c r="F182" s="21"/>
       <c r="G182" s="21"/>
       <c r="H182" s="21"/>
-      <c r="I182" s="21"/>
-    </row>
-    <row r="183" spans="3:9" hidden="1" outlineLevel="1">
+      <c r="I182" s="21" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="183" spans="3:9" outlineLevel="1">
       <c r="C183" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D183" s="21"/>
       <c r="E183" s="21"/>
       <c r="F183" s="21"/>
       <c r="G183" s="21"/>
       <c r="H183" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="I183" s="21"/>
+    </row>
+    <row r="184" spans="3:9" outlineLevel="1">
+      <c r="C184" s="15" t="s">
         <v>214</v>
-      </c>
-      <c r="I183" s="21"/>
-    </row>
-    <row r="184" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C184" s="15" t="s">
-        <v>215</v>
       </c>
       <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="21"/>
       <c r="G184" s="21"/>
       <c r="H184" s="21"/>
-      <c r="I184" s="21"/>
-    </row>
-    <row r="185" spans="3:9" hidden="1" outlineLevel="1">
+      <c r="I184" s="21" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="185" spans="3:9" outlineLevel="1">
       <c r="D185" s="38"/>
       <c r="E185" s="38"/>
       <c r="F185" s="38"/>
@@ -4272,7 +4305,7 @@
       <c r="H185" s="38"/>
       <c r="I185" s="38"/>
     </row>
-    <row r="186" spans="3:9" collapsed="1">
+    <row r="186" spans="3:9">
       <c r="C186" s="26"/>
       <c r="D186" s="38"/>
       <c r="E186" s="38"/>
@@ -4283,7 +4316,7 @@
     </row>
     <row r="187" spans="3:9">
       <c r="C187" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D187" s="38"/>
       <c r="E187" s="38"/>
@@ -4292,20 +4325,20 @@
       <c r="H187" s="38"/>
       <c r="I187" s="38"/>
     </row>
-    <row r="188" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="188" spans="3:9" outlineLevel="1">
       <c r="C188" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D188" s="21"/>
       <c r="E188" s="21"/>
       <c r="F188" s="21"/>
       <c r="G188" s="21"/>
       <c r="H188" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I188" s="21"/>
     </row>
-    <row r="189" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="189" spans="3:9" outlineLevel="1">
       <c r="C189" s="22"/>
       <c r="D189" s="38"/>
       <c r="E189" s="38"/>
@@ -4314,9 +4347,9 @@
       <c r="H189" s="38"/>
       <c r="I189" s="38"/>
     </row>
-    <row r="190" spans="3:9" collapsed="1">
+    <row r="190" spans="3:9">
       <c r="C190" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D190" s="38"/>
       <c r="E190" s="38"/>
@@ -4327,7 +4360,7 @@
     </row>
     <row r="191" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C191" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D191" s="21"/>
       <c r="E191" s="21"/>
@@ -4335,12 +4368,12 @@
       <c r="G191" s="21"/>
       <c r="H191" s="21"/>
       <c r="I191" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="192" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C192" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D192" s="21"/>
       <c r="E192" s="21"/>
@@ -4348,12 +4381,12 @@
       <c r="G192" s="21"/>
       <c r="H192" s="21"/>
       <c r="I192" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="193" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C193" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D193" s="21"/>
       <c r="E193" s="21"/>
@@ -4361,12 +4394,12 @@
       <c r="G193" s="21"/>
       <c r="H193" s="21"/>
       <c r="I193" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="194" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C194" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D194" s="21"/>
       <c r="E194" s="21"/>
@@ -4374,12 +4407,12 @@
       <c r="G194" s="21"/>
       <c r="H194" s="21"/>
       <c r="I194" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="195" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C195" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D195" s="21"/>
       <c r="E195" s="21"/>
@@ -4387,12 +4420,12 @@
       <c r="G195" s="21"/>
       <c r="H195" s="21"/>
       <c r="I195" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="196" spans="3:9" hidden="1" outlineLevel="1">
       <c r="C196" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D196" s="21"/>
       <c r="E196" s="21"/>
@@ -4400,7 +4433,7 @@
       <c r="G196" s="21"/>
       <c r="H196" s="21"/>
       <c r="I196" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" spans="3:9" hidden="1" outlineLevel="1">
@@ -4414,7 +4447,7 @@
     </row>
     <row r="198" spans="3:9" collapsed="1">
       <c r="C198" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D198" s="38"/>
       <c r="E198" s="38"/>
@@ -4423,9 +4456,9 @@
       <c r="H198" s="38"/>
       <c r="I198" s="38"/>
     </row>
-    <row r="199" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="199" spans="3:9" outlineLevel="1">
       <c r="C199" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D199" s="21"/>
       <c r="E199" s="21"/>
@@ -4433,12 +4466,12 @@
       <c r="G199" s="21"/>
       <c r="H199" s="21"/>
       <c r="I199" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="200" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="200" spans="3:9" outlineLevel="1">
       <c r="C200" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D200" s="21"/>
       <c r="E200" s="21"/>
@@ -4446,12 +4479,12 @@
       <c r="G200" s="21"/>
       <c r="H200" s="21"/>
       <c r="I200" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="201" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="201" spans="3:9" outlineLevel="1">
       <c r="C201" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D201" s="21"/>
       <c r="E201" s="21"/>
@@ -4459,12 +4492,12 @@
       <c r="G201" s="21"/>
       <c r="H201" s="21"/>
       <c r="I201" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="202" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="202" spans="3:9" outlineLevel="1">
       <c r="C202" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D202" s="21"/>
       <c r="E202" s="21"/>
@@ -4472,12 +4505,12 @@
       <c r="G202" s="21"/>
       <c r="H202" s="21"/>
       <c r="I202" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="203" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="203" spans="3:9" outlineLevel="1">
       <c r="C203" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D203" s="21"/>
       <c r="E203" s="21"/>
@@ -4486,7 +4519,7 @@
       <c r="H203" s="21"/>
       <c r="I203" s="21"/>
     </row>
-    <row r="204" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="204" spans="3:9" outlineLevel="1">
       <c r="C204" s="24"/>
       <c r="D204" s="38"/>
       <c r="E204" s="38"/>
@@ -4495,7 +4528,7 @@
       <c r="H204" s="38"/>
       <c r="I204" s="38"/>
     </row>
-    <row r="205" spans="3:9" collapsed="1">
+    <row r="205" spans="3:9">
       <c r="D205" s="38"/>
       <c r="E205" s="38"/>
       <c r="F205" s="38"/>
@@ -4505,7 +4538,7 @@
     </row>
     <row r="206" spans="3:9">
       <c r="C206" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D206" s="38"/>
       <c r="E206" s="38"/>
@@ -4514,9 +4547,9 @@
       <c r="H206" s="38"/>
       <c r="I206" s="38"/>
     </row>
-    <row r="207" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="207" spans="3:9" outlineLevel="1">
       <c r="C207" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D207" s="21"/>
       <c r="E207" s="21"/>
@@ -4524,26 +4557,26 @@
       <c r="G207" s="21"/>
       <c r="H207" s="21"/>
       <c r="I207" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="208" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="208" spans="3:9" outlineLevel="1">
       <c r="C208" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D208" s="21"/>
       <c r="E208" s="21"/>
       <c r="F208" s="21"/>
       <c r="G208" s="21"/>
       <c r="H208" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I208" s="21"/>
     </row>
-    <row r="209" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="209" spans="2:9" outlineLevel="1">
       <c r="B209" s="5"/>
       <c r="C209" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D209" s="21"/>
       <c r="E209" s="21"/>
@@ -4551,13 +4584,13 @@
       <c r="G209" s="21"/>
       <c r="H209" s="21"/>
       <c r="I209" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="210" spans="2:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" outlineLevel="1">
       <c r="B210" s="5"/>
       <c r="C210" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D210" s="21"/>
       <c r="E210" s="21"/>
@@ -4565,28 +4598,28 @@
       <c r="G210" s="21"/>
       <c r="H210" s="21"/>
       <c r="I210" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="211" spans="2:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" outlineLevel="1">
       <c r="C211" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D211" s="21"/>
       <c r="E211" s="21"/>
       <c r="F211" s="21"/>
       <c r="G211" s="21"/>
       <c r="H211" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I211" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="I211" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="212" spans="2:9" hidden="1" outlineLevel="1">
+    </row>
+    <row r="212" spans="2:9" outlineLevel="1">
       <c r="B212" s="5"/>
       <c r="C212" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D212" s="21"/>
       <c r="E212" s="21"/>
@@ -4594,10 +4627,10 @@
       <c r="G212" s="21"/>
       <c r="H212" s="21"/>
       <c r="I212" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="213" spans="2:9" hidden="1" outlineLevel="1">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" outlineLevel="1">
       <c r="B213" s="5"/>
       <c r="C213" s="32"/>
       <c r="D213" s="38"/>
@@ -4607,9 +4640,9 @@
       <c r="H213" s="38"/>
       <c r="I213" s="38"/>
     </row>
-    <row r="214" spans="2:9" collapsed="1">
+    <row r="214" spans="2:9">
       <c r="C214" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D214" s="38"/>
       <c r="E214" s="38"/>
@@ -4620,7 +4653,7 @@
     </row>
     <row r="215" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C215" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D215" s="21"/>
       <c r="E215" s="21"/>
@@ -4628,12 +4661,12 @@
       <c r="G215" s="21"/>
       <c r="H215" s="21"/>
       <c r="I215" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="216" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C216" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D216" s="21"/>
       <c r="E216" s="21"/>
@@ -4641,12 +4674,12 @@
       <c r="G216" s="21"/>
       <c r="H216" s="21"/>
       <c r="I216" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="217" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C217" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D217" s="21"/>
       <c r="E217" s="21"/>
@@ -4654,38 +4687,38 @@
       <c r="G217" s="21"/>
       <c r="H217" s="21"/>
       <c r="I217" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="218" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C218" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D218" s="21"/>
       <c r="E218" s="21"/>
       <c r="F218" s="21"/>
       <c r="G218" s="21"/>
       <c r="H218" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I218" s="21"/>
     </row>
     <row r="219" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C219" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D219" s="21"/>
       <c r="E219" s="21"/>
       <c r="F219" s="21"/>
       <c r="G219" s="21"/>
       <c r="H219" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I219" s="21"/>
     </row>
     <row r="220" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C220" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D220" s="21"/>
       <c r="E220" s="21"/>
@@ -4693,12 +4726,12 @@
       <c r="G220" s="21"/>
       <c r="H220" s="21"/>
       <c r="I220" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="221" spans="2:9" hidden="1" outlineLevel="1">
       <c r="C221" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D221" s="21"/>
       <c r="E221" s="21"/>
@@ -4706,7 +4739,7 @@
       <c r="G221" s="21"/>
       <c r="H221" s="21"/>
       <c r="I221" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="222" spans="2:9" hidden="1" outlineLevel="1">
@@ -4720,7 +4753,7 @@
     </row>
     <row r="223" spans="2:9" collapsed="1">
       <c r="C223" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D223" s="38"/>
       <c r="E223" s="38"/>
@@ -4729,9 +4762,9 @@
       <c r="H223" s="38"/>
       <c r="I223" s="38"/>
     </row>
-    <row r="224" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="224" spans="2:9" outlineLevel="1">
       <c r="C224" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D224" s="21"/>
       <c r="E224" s="21"/>
@@ -4739,12 +4772,12 @@
       <c r="G224" s="21"/>
       <c r="H224" s="21"/>
       <c r="I224" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="225" spans="3:9" hidden="1" outlineLevel="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="225" spans="3:9" outlineLevel="1">
       <c r="C225" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D225" s="21"/>
       <c r="E225" s="21"/>
@@ -4752,12 +4785,12 @@
       <c r="G225" s="21"/>
       <c r="H225" s="21"/>
       <c r="I225" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="226" spans="3:9" outlineLevel="1">
+      <c r="C226" s="15" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="226" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C226" s="15" t="s">
-        <v>257</v>
       </c>
       <c r="D226" s="21"/>
       <c r="E226" s="21"/>
@@ -4765,12 +4798,12 @@
       <c r="G226" s="21"/>
       <c r="H226" s="21"/>
       <c r="I226" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="227" spans="3:9" hidden="1" outlineLevel="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="227" spans="3:9" outlineLevel="1">
       <c r="C227" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D227" s="21"/>
       <c r="E227" s="21"/>
@@ -4778,12 +4811,12 @@
       <c r="G227" s="21"/>
       <c r="H227" s="21"/>
       <c r="I227" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="228" spans="3:9" hidden="1" outlineLevel="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="228" spans="3:9" outlineLevel="1">
       <c r="C228" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D228" s="21"/>
       <c r="E228" s="21"/>
@@ -4791,58 +4824,57 @@
       <c r="G228" s="21"/>
       <c r="H228" s="21"/>
       <c r="I228" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="229" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="230" spans="3:9" collapsed="1"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="229" spans="3:9" outlineLevel="1"/>
     <row r="231" spans="3:9">
       <c r="C231" s="20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="232" spans="3:9" outlineLevel="1">
+      <c r="C232" s="3" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="232" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C232" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="D232" s="21"/>
       <c r="E232" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F232" s="21"/>
       <c r="G232" s="21"/>
       <c r="H232" s="21"/>
       <c r="I232" s="21"/>
     </row>
-    <row r="233" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="233" spans="3:9" outlineLevel="1">
       <c r="C233" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D233" s="21"/>
       <c r="E233" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F233" s="21"/>
       <c r="G233" s="21"/>
       <c r="H233" s="21"/>
       <c r="I233" s="21"/>
     </row>
-    <row r="234" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="234" spans="3:9" outlineLevel="1">
       <c r="C234" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D234" s="21"/>
       <c r="E234" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F234" s="21"/>
       <c r="G234" s="21"/>
       <c r="H234" s="21"/>
       <c r="I234" s="21"/>
     </row>
-    <row r="235" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="235" spans="3:9" outlineLevel="1">
       <c r="C235" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D235" s="21"/>
       <c r="E235" s="21"/>
@@ -4850,12 +4882,12 @@
       <c r="G235" s="21"/>
       <c r="H235" s="21"/>
       <c r="I235" s="21" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="236" spans="3:9" outlineLevel="1">
+      <c r="C236" s="3" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="236" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C236" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="D236" s="21"/>
       <c r="E236" s="21"/>
@@ -4863,12 +4895,12 @@
       <c r="G236" s="21"/>
       <c r="H236" s="21"/>
       <c r="I236" s="21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="237" spans="3:9" hidden="1" outlineLevel="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="237" spans="3:9" outlineLevel="1">
       <c r="C237" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D237" s="21"/>
       <c r="E237" s="21"/>
@@ -4876,12 +4908,12 @@
       <c r="G237" s="21"/>
       <c r="H237" s="21"/>
       <c r="I237" s="21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="238" spans="3:9" hidden="1" outlineLevel="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="238" spans="3:9" outlineLevel="1">
       <c r="C238" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D238" s="21"/>
       <c r="E238" s="21"/>
@@ -4889,210 +4921,210 @@
       <c r="G238" s="21"/>
       <c r="H238" s="21"/>
       <c r="I238" s="21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="239" spans="3:9" hidden="1" outlineLevel="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="239" spans="3:9" outlineLevel="1">
       <c r="C239" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D239" s="21"/>
       <c r="E239" s="21"/>
       <c r="F239" s="21"/>
       <c r="G239" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H239" s="21"/>
       <c r="I239" s="21"/>
     </row>
-    <row r="240" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="240" spans="3:9" outlineLevel="1">
       <c r="C240" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D240" s="21"/>
       <c r="E240" s="21"/>
       <c r="F240" s="21"/>
       <c r="G240" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H240" s="21"/>
       <c r="I240" s="21"/>
     </row>
-    <row r="241" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="241" spans="3:9" outlineLevel="1">
       <c r="C241" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D241" s="21"/>
       <c r="E241" s="21"/>
       <c r="F241" s="21"/>
       <c r="G241" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H241" s="21"/>
       <c r="I241" s="21"/>
     </row>
-    <row r="242" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="242" spans="3:9" outlineLevel="1">
       <c r="C242" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D242" s="21"/>
       <c r="E242" s="21"/>
       <c r="F242" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G242" s="21"/>
       <c r="H242" s="21"/>
       <c r="I242" s="21"/>
     </row>
-    <row r="243" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="243" spans="3:9" outlineLevel="1">
       <c r="C243" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D243" s="21"/>
       <c r="E243" s="21"/>
       <c r="F243" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G243" s="21"/>
       <c r="H243" s="21"/>
       <c r="I243" s="21"/>
     </row>
-    <row r="244" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="244" spans="3:9" outlineLevel="1">
       <c r="C244" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D244" s="21"/>
       <c r="E244" s="21"/>
       <c r="F244" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G244" s="21"/>
       <c r="H244" s="21"/>
       <c r="I244" s="21"/>
     </row>
-    <row r="245" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="245" spans="3:9" outlineLevel="1">
       <c r="C245" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D245" s="21"/>
       <c r="E245" s="21"/>
       <c r="F245" s="21"/>
       <c r="G245" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H245" s="21"/>
       <c r="I245" s="21"/>
     </row>
-    <row r="246" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="246" spans="3:9" outlineLevel="1">
       <c r="C246" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D246" s="21"/>
       <c r="E246" s="21"/>
       <c r="F246" s="21"/>
       <c r="G246" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H246" s="21"/>
       <c r="I246" s="21"/>
     </row>
-    <row r="247" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="247" spans="3:9" outlineLevel="1">
       <c r="C247" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D247" s="21"/>
       <c r="E247" s="21"/>
       <c r="F247" s="21"/>
       <c r="G247" s="21"/>
       <c r="H247" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="I247" s="21"/>
+    </row>
+    <row r="248" spans="3:9" outlineLevel="1">
+      <c r="C248" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="I247" s="21"/>
-    </row>
-    <row r="248" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C248" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="D248" s="21"/>
       <c r="E248" s="21"/>
       <c r="F248" s="21"/>
       <c r="G248" s="21"/>
       <c r="H248" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I248" s="21"/>
     </row>
-    <row r="249" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="249" spans="3:9" outlineLevel="1">
       <c r="C249" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D249" s="21"/>
       <c r="E249" s="21"/>
       <c r="F249" s="21"/>
       <c r="G249" s="21"/>
       <c r="H249" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="I249" s="21"/>
+    </row>
+    <row r="250" spans="3:9" outlineLevel="1">
+      <c r="C250" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="I249" s="21"/>
-    </row>
-    <row r="250" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C250" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="D250" s="21"/>
       <c r="E250" s="21"/>
       <c r="F250" s="21"/>
       <c r="G250" s="21"/>
       <c r="H250" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I250" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="251" spans="3:9" hidden="1" outlineLevel="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="251" spans="3:9" outlineLevel="1">
       <c r="C251" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="D251" s="21" t="s">
         <v>290</v>
-      </c>
-      <c r="D251" s="21" t="s">
-        <v>291</v>
       </c>
       <c r="E251" s="21"/>
       <c r="F251" s="21"/>
       <c r="G251" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H251" s="21"/>
       <c r="I251" s="21"/>
     </row>
-    <row r="252" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="252" spans="3:9" outlineLevel="1">
       <c r="D252" s="32"/>
     </row>
-    <row r="253" spans="3:9" collapsed="1">
+    <row r="253" spans="3:9">
       <c r="D253" s="32"/>
     </row>
     <row r="254" spans="3:9">
       <c r="C254" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D254" s="32"/>
+    </row>
+    <row r="255" spans="3:9" outlineLevel="1">
+      <c r="C255" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="D254" s="32"/>
-    </row>
-    <row r="255" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C255" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="D255" s="21"/>
       <c r="E255" s="21"/>
       <c r="F255" s="21"/>
       <c r="G255" s="21"/>
       <c r="H255" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I255" s="21"/>
     </row>
-    <row r="256" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="256" spans="3:9" outlineLevel="1">
       <c r="C256" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D256" s="21"/>
       <c r="E256" s="21"/>
@@ -5100,109 +5132,108 @@
       <c r="G256" s="21"/>
       <c r="H256" s="21"/>
       <c r="I256" s="21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="257" spans="3:9" hidden="1" outlineLevel="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="257" spans="3:9" outlineLevel="1">
       <c r="C257" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D257" s="21"/>
       <c r="E257" s="21"/>
       <c r="F257" s="21"/>
       <c r="G257" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H257" s="21"/>
       <c r="I257" s="21"/>
     </row>
-    <row r="258" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="258" spans="3:9" outlineLevel="1">
       <c r="D258" s="32"/>
     </row>
-    <row r="259" spans="3:9" collapsed="1">
+    <row r="259" spans="3:9">
       <c r="D259" s="32"/>
     </row>
     <row r="260" spans="3:9">
       <c r="C260" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="D260" s="32"/>
+    </row>
+    <row r="261" spans="3:9" outlineLevel="1">
+      <c r="C261" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="D260" s="32"/>
-    </row>
-    <row r="261" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C261" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="D261" s="21"/>
       <c r="E261" s="21"/>
       <c r="F261" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G261" s="21"/>
       <c r="H261" s="21"/>
       <c r="I261" s="21"/>
     </row>
-    <row r="262" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="262" spans="3:9" outlineLevel="1">
       <c r="C262" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D262" s="21"/>
       <c r="E262" s="21"/>
       <c r="F262" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G262" s="21"/>
       <c r="H262" s="21"/>
       <c r="I262" s="21"/>
     </row>
-    <row r="263" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="263" spans="3:9" outlineLevel="1">
       <c r="C263" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D263" s="21"/>
       <c r="E263" s="21"/>
       <c r="F263" s="21"/>
       <c r="G263" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H263" s="21"/>
       <c r="I263" s="21"/>
     </row>
-    <row r="264" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="264" spans="3:9" outlineLevel="1">
       <c r="C264" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D264" s="21"/>
       <c r="E264" s="21"/>
       <c r="F264" s="21"/>
       <c r="G264" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H264" s="21"/>
       <c r="I264" s="21"/>
     </row>
-    <row r="265" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="265" spans="3:9" outlineLevel="1">
       <c r="C265" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D265" s="21"/>
       <c r="E265" s="21"/>
       <c r="F265" s="21"/>
       <c r="G265" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H265" s="21"/>
       <c r="I265" s="21"/>
     </row>
-    <row r="266" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="267" spans="3:9" collapsed="1"/>
+    <row r="266" spans="3:9" outlineLevel="1"/>
     <row r="268" spans="3:9">
       <c r="C268" s="29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="269" spans="3:9" outlineLevel="1">
+      <c r="C269" s="12" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="269" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C269" s="12" t="s">
-        <v>305</v>
       </c>
       <c r="D269" s="21"/>
       <c r="E269" s="21"/>
@@ -5210,12 +5241,12 @@
       <c r="G269" s="21"/>
       <c r="H269" s="21"/>
       <c r="I269" s="21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="270" spans="3:9" outlineLevel="1">
+      <c r="C270" s="3" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="270" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C270" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="D270" s="21"/>
       <c r="E270" s="21"/>
@@ -5223,12 +5254,12 @@
       <c r="G270" s="21"/>
       <c r="H270" s="21"/>
       <c r="I270" s="21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="271" spans="3:9" outlineLevel="1">
+      <c r="C271" s="14" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="271" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C271" s="14" t="s">
-        <v>309</v>
       </c>
       <c r="D271" s="21"/>
       <c r="E271" s="21"/>
@@ -5236,20 +5267,19 @@
       <c r="G271" s="21"/>
       <c r="H271" s="21"/>
       <c r="I271" s="21" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="272" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="273" spans="2:9" collapsed="1"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="272" spans="3:9" outlineLevel="1"/>
     <row r="274" spans="2:9">
       <c r="B274" s="7"/>
       <c r="C274" s="29" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="275" spans="2:9" outlineLevel="1">
+      <c r="C275" s="3" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="275" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C275" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="D275" s="21"/>
       <c r="E275" s="21"/>
@@ -5257,42 +5287,42 @@
       <c r="G275" s="21"/>
       <c r="H275" s="21"/>
       <c r="I275" s="21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="276" spans="2:9" outlineLevel="1">
+      <c r="C276" s="3" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="276" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C276" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="D276" s="21"/>
       <c r="E276" s="21"/>
       <c r="F276" s="21"/>
       <c r="G276" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H276" s="21"/>
       <c r="I276" s="21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="277" spans="2:9" hidden="1" outlineLevel="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="277" spans="2:9" outlineLevel="1">
       <c r="C277" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D277" s="21"/>
       <c r="E277" s="21"/>
       <c r="F277" s="21"/>
       <c r="G277" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H277" s="21"/>
       <c r="I277" s="21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="278" spans="2:9" hidden="1" outlineLevel="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="278" spans="2:9" outlineLevel="1">
       <c r="C278" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D278" s="21"/>
       <c r="E278" s="21"/>
@@ -5300,12 +5330,12 @@
       <c r="G278" s="21"/>
       <c r="H278" s="21"/>
       <c r="I278" s="21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="279" spans="2:9" hidden="1" outlineLevel="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="279" spans="2:9" outlineLevel="1">
       <c r="C279" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D279" s="21"/>
       <c r="E279" s="21"/>
@@ -5313,12 +5343,12 @@
       <c r="G279" s="21"/>
       <c r="H279" s="21"/>
       <c r="I279" s="21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="280" spans="2:9" hidden="1" outlineLevel="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="280" spans="2:9" outlineLevel="1">
       <c r="C280" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D280" s="21"/>
       <c r="E280" s="21"/>
@@ -5327,34 +5357,34 @@
       <c r="H280" s="21"/>
       <c r="I280" s="21"/>
     </row>
-    <row r="281" spans="2:9" hidden="1" outlineLevel="1"/>
-    <row r="282" spans="2:9" collapsed="1">
+    <row r="281" spans="2:9" outlineLevel="1"/>
+    <row r="282" spans="2:9">
       <c r="B282" s="7"/>
     </row>
     <row r="283" spans="2:9">
       <c r="B283" s="7"/>
       <c r="C283" s="29" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="284" spans="2:9" outlineLevel="1">
+      <c r="C284" s="15" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="284" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C284" s="15" t="s">
+      <c r="D284" s="21" t="s">
         <v>319</v>
-      </c>
-      <c r="D284" s="21" t="s">
-        <v>320</v>
       </c>
       <c r="E284" s="21"/>
       <c r="F284" s="21"/>
       <c r="G284" s="21"/>
       <c r="H284" s="21"/>
       <c r="I284" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="285" spans="2:9" outlineLevel="1">
+      <c r="C285" s="15" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="285" spans="2:9" hidden="1" outlineLevel="1">
-      <c r="C285" s="15" t="s">
-        <v>322</v>
       </c>
       <c r="D285" s="21"/>
       <c r="E285" s="21"/>
@@ -5363,308 +5393,306 @@
       <c r="H285" s="21"/>
       <c r="I285" s="21"/>
     </row>
-    <row r="286" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="286" spans="2:9" outlineLevel="1">
       <c r="C286" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D286" s="21"/>
       <c r="E286" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F286" s="21"/>
       <c r="G286" s="21"/>
       <c r="H286" s="21"/>
       <c r="I286" s="21"/>
     </row>
-    <row r="287" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="287" spans="2:9" outlineLevel="1">
       <c r="C287" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D287" s="21" t="s">
         <v>325</v>
       </c>
-      <c r="D287" s="21" t="s">
-        <v>326</v>
-      </c>
       <c r="E287" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F287" s="21"/>
       <c r="G287" s="21"/>
       <c r="H287" s="21"/>
       <c r="I287" s="21"/>
     </row>
-    <row r="288" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="288" spans="2:9" outlineLevel="1">
       <c r="C288" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D288" s="21"/>
       <c r="E288" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F288" s="21"/>
       <c r="G288" s="21"/>
       <c r="H288" s="21"/>
       <c r="I288" s="21"/>
     </row>
-    <row r="289" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="289" spans="3:9" outlineLevel="1">
       <c r="C289" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D289" s="21"/>
       <c r="E289" s="21"/>
       <c r="F289" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G289" s="21"/>
       <c r="H289" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="I289" s="21"/>
+    </row>
+    <row r="290" spans="3:9" outlineLevel="1">
+      <c r="C290" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="I289" s="21"/>
-    </row>
-    <row r="290" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C290" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="D290" s="21"/>
       <c r="E290" s="21"/>
       <c r="F290" s="21"/>
       <c r="G290" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H290" s="21"/>
       <c r="I290" s="21"/>
     </row>
-    <row r="291" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="291" spans="3:9" outlineLevel="1">
       <c r="C291" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D291" s="21"/>
       <c r="E291" s="21"/>
       <c r="F291" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G291" s="21"/>
       <c r="H291" s="21"/>
       <c r="I291" s="21"/>
     </row>
-    <row r="292" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="292" spans="3:9" outlineLevel="1">
       <c r="C292" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D292" s="21"/>
       <c r="E292" s="21"/>
       <c r="F292" s="21"/>
       <c r="G292" s="21"/>
       <c r="H292" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I292" s="21"/>
     </row>
-    <row r="293" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="293" spans="3:9" outlineLevel="1">
       <c r="C293" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D293" s="21"/>
       <c r="E293" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F293" s="21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G293" s="21"/>
       <c r="H293" s="21"/>
       <c r="I293" s="21"/>
     </row>
-    <row r="294" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="294" spans="3:9" outlineLevel="1">
       <c r="C294" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D294" s="21"/>
       <c r="E294" s="21"/>
       <c r="F294" s="21"/>
       <c r="G294" s="21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H294" s="21"/>
       <c r="I294" s="21"/>
     </row>
-    <row r="295" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="295" spans="3:9" outlineLevel="1">
       <c r="C295" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D295" s="21"/>
       <c r="E295" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F295" s="21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G295" s="21"/>
       <c r="H295" s="21"/>
       <c r="I295" s="21"/>
     </row>
-    <row r="296" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="296" spans="3:9" outlineLevel="1">
       <c r="C296" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D296" s="21"/>
       <c r="E296" s="21"/>
       <c r="F296" s="21"/>
       <c r="G296" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H296" s="21"/>
       <c r="I296" s="21"/>
     </row>
-    <row r="297" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="297" spans="3:9" outlineLevel="1">
       <c r="C297" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D297" s="21"/>
       <c r="E297" s="21"/>
       <c r="F297" s="21"/>
       <c r="G297" s="21"/>
       <c r="H297" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="I297" s="21"/>
+    </row>
+    <row r="298" spans="3:9" outlineLevel="1">
+      <c r="C298" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="I297" s="21"/>
-    </row>
-    <row r="298" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C298" s="3" t="s">
-        <v>345</v>
       </c>
       <c r="D298" s="21"/>
       <c r="E298" s="21"/>
       <c r="F298" s="21"/>
       <c r="G298" s="21"/>
       <c r="H298" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I298" s="21"/>
     </row>
-    <row r="299" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="299" spans="3:9" outlineLevel="1">
       <c r="C299" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D299" s="21"/>
       <c r="E299" s="21"/>
       <c r="F299" s="21"/>
       <c r="G299" s="21"/>
       <c r="H299" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="I299" s="21"/>
+    </row>
+    <row r="300" spans="3:9" outlineLevel="1">
+      <c r="C300" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="I299" s="21"/>
-    </row>
-    <row r="300" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C300" s="3" t="s">
-        <v>348</v>
       </c>
       <c r="D300" s="21"/>
       <c r="E300" s="21"/>
       <c r="F300" s="21"/>
       <c r="G300" s="21"/>
       <c r="H300" s="21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I300" s="21"/>
     </row>
-    <row r="301" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="302" spans="3:9" collapsed="1"/>
+    <row r="301" spans="3:9" outlineLevel="1"/>
     <row r="303" spans="3:9">
       <c r="C303" s="30" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="304" spans="3:9" outlineLevel="1">
+      <c r="C304" s="28" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="304" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C304" s="28" t="s">
-        <v>350</v>
       </c>
       <c r="D304" s="21"/>
       <c r="E304" s="21"/>
       <c r="F304" s="21"/>
       <c r="G304" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H304" s="21"/>
       <c r="I304" s="21"/>
     </row>
-    <row r="305" spans="3:9" ht="30" hidden="1" outlineLevel="1">
+    <row r="305" spans="3:9" ht="28" outlineLevel="1">
       <c r="C305" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D305" s="21"/>
       <c r="E305" s="21"/>
       <c r="F305" s="21"/>
       <c r="G305" s="21"/>
       <c r="H305" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="I305" s="21"/>
+    </row>
+    <row r="306" spans="3:9" outlineLevel="1">
+      <c r="C306" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="I305" s="21"/>
-    </row>
-    <row r="306" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C306" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="D306" s="21"/>
       <c r="E306" s="21"/>
       <c r="F306" s="21"/>
       <c r="G306" s="21"/>
       <c r="H306" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I306" s="21"/>
     </row>
-    <row r="307" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="307" spans="3:9" outlineLevel="1">
       <c r="C307" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D307" s="21"/>
       <c r="E307" s="21"/>
       <c r="F307" s="21"/>
       <c r="G307" s="21"/>
       <c r="H307" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="I307" s="21"/>
+    </row>
+    <row r="308" spans="3:9" outlineLevel="1">
+      <c r="C308" s="31" t="s">
         <v>356</v>
-      </c>
-      <c r="I307" s="21"/>
-    </row>
-    <row r="308" spans="3:9" ht="26.25" hidden="1" outlineLevel="1">
-      <c r="C308" s="31" t="s">
-        <v>357</v>
       </c>
       <c r="D308" s="21"/>
       <c r="E308" s="21"/>
       <c r="F308" s="21"/>
       <c r="G308" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H308" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="I308" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="I308" s="21" t="s">
+    </row>
+    <row r="309" spans="3:9" outlineLevel="1">
+      <c r="C309" s="3" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="309" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C309" s="3" t="s">
-        <v>360</v>
       </c>
       <c r="D309" s="21"/>
       <c r="E309" s="21"/>
       <c r="F309" s="21"/>
       <c r="G309" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H309" s="21"/>
       <c r="I309" s="21"/>
     </row>
-    <row r="310" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="311" spans="3:9" collapsed="1"/>
+    <row r="310" spans="3:9" outlineLevel="1"/>
     <row r="312" spans="3:9">
       <c r="C312" s="29" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="313" spans="3:9" outlineLevel="1">
+      <c r="C313" s="3" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="313" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C313" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="D313" s="21"/>
       <c r="E313" s="21"/>
@@ -5672,12 +5700,12 @@
       <c r="G313" s="21"/>
       <c r="H313" s="21"/>
       <c r="I313" s="21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="314" spans="3:9" outlineLevel="1">
+      <c r="C314" s="3" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="314" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C314" s="3" t="s">
-        <v>364</v>
       </c>
       <c r="D314" s="21"/>
       <c r="E314" s="21"/>
@@ -5685,78 +5713,76 @@
       <c r="G314" s="21"/>
       <c r="H314" s="21"/>
       <c r="I314" s="21" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="315" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="316" spans="3:9" collapsed="1"/>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="315" spans="3:9" outlineLevel="1"/>
     <row r="317" spans="3:9">
       <c r="C317" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="318" spans="3:9" outlineLevel="1">
+      <c r="C318" s="11" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="318" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C318" s="11" t="s">
-        <v>366</v>
       </c>
       <c r="D318" s="21"/>
       <c r="E318" s="21"/>
       <c r="F318" s="21"/>
       <c r="G318" s="21"/>
       <c r="H318" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="I318" s="21"/>
+    </row>
+    <row r="319" spans="3:9" outlineLevel="1">
+      <c r="C319" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="I318" s="21"/>
-    </row>
-    <row r="319" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C319" s="3" t="s">
-        <v>368</v>
       </c>
       <c r="D319" s="21"/>
       <c r="E319" s="21"/>
       <c r="F319" s="21"/>
       <c r="G319" s="21"/>
       <c r="H319" s="21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I319" s="21"/>
     </row>
-    <row r="320" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="320" spans="3:9" outlineLevel="1">
       <c r="C320" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D320" s="21"/>
       <c r="E320" s="21"/>
       <c r="F320" s="21"/>
       <c r="G320" s="21"/>
       <c r="H320" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="I320" s="21"/>
+    </row>
+    <row r="321" spans="3:9" outlineLevel="1">
+      <c r="C321" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="I320" s="21"/>
-    </row>
-    <row r="321" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C321" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="D321" s="21"/>
       <c r="E321" s="21"/>
       <c r="F321" s="21"/>
       <c r="G321" s="21"/>
       <c r="H321" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I321" s="21"/>
     </row>
-    <row r="322" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="323" spans="3:9" collapsed="1"/>
+    <row r="322" spans="3:9" outlineLevel="1"/>
     <row r="324" spans="3:9">
       <c r="C324" s="29" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="325" spans="3:9" outlineLevel="1">
+      <c r="C325" s="3" t="s">
         <v>372</v>
-      </c>
-    </row>
-    <row r="325" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C325" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="D325" s="21"/>
       <c r="E325" s="21"/>
@@ -5764,12 +5790,12 @@
       <c r="G325" s="21"/>
       <c r="H325" s="21"/>
       <c r="I325" s="21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="326" spans="3:9" outlineLevel="1">
+      <c r="C326" s="3" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="326" spans="3:9" hidden="1" outlineLevel="1">
-      <c r="C326" s="3" t="s">
-        <v>375</v>
       </c>
       <c r="D326" s="21"/>
       <c r="E326" s="21"/>
@@ -5777,13 +5803,17 @@
       <c r="G326" s="21"/>
       <c r="H326" s="21"/>
       <c r="I326" s="21" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="327" spans="3:9" hidden="1" outlineLevel="1"/>
-    <row r="328" spans="3:9" collapsed="1"/>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="327" spans="3:9" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated sheet with standards-first view
</commit_message>
<xml_diff>
--- a/K5Mathlearningobjectives.xlsx
+++ b/K5Mathlearningobjectives.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="620" windowWidth="24440" windowHeight="15600"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="22460" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Update 9_30_15" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="381">
   <si>
     <t>Open Learning Objectives: K-5 math</t>
   </si>
@@ -1325,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="197">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1522,6 +1522,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
@@ -1621,7 +1627,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="197">
+  <cellStyles count="203">
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
@@ -1732,6 +1738,9 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
@@ -1818,6 +1827,9 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2123,15 +2135,15 @@
   <dimension ref="B2:I327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I185" sqref="I185"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="4" style="8" customWidth="1"/>
-    <col min="3" max="3" width="114.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.5" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" style="25" bestFit="1" customWidth="1"/>
@@ -2827,7 +2839,9 @@
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
+      <c r="F56" s="21" t="s">
+        <v>376</v>
+      </c>
       <c r="G56" s="21"/>
       <c r="H56" s="21"/>
       <c r="I56" s="21"/>
@@ -3033,7 +3047,9 @@
       <c r="E71" s="21"/>
       <c r="F71" s="21"/>
       <c r="G71" s="21"/>
-      <c r="H71" s="21"/>
+      <c r="H71" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="I71" s="21"/>
     </row>
     <row r="72" spans="2:9" outlineLevel="1"/>
@@ -3912,7 +3928,7 @@
       </c>
       <c r="I153" s="21"/>
     </row>
-    <row r="154" spans="2:9" ht="28" outlineLevel="1">
+    <row r="154" spans="2:9" ht="42" outlineLevel="1">
       <c r="C154" s="23" t="s">
         <v>175</v>
       </c>
@@ -4358,7 +4374,7 @@
       <c r="H190" s="38"/>
       <c r="I190" s="38"/>
     </row>
-    <row r="191" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="191" spans="3:9" outlineLevel="1">
       <c r="C191" s="9" t="s">
         <v>219</v>
       </c>
@@ -4371,7 +4387,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="192" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="192" spans="3:9" outlineLevel="1">
       <c r="C192" s="9" t="s">
         <v>221</v>
       </c>
@@ -4384,7 +4400,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="193" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="193" spans="3:9" outlineLevel="1">
       <c r="C193" s="9" t="s">
         <v>222</v>
       </c>
@@ -4397,7 +4413,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="194" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="194" spans="3:9" outlineLevel="1">
       <c r="C194" s="9" t="s">
         <v>223</v>
       </c>
@@ -4410,7 +4426,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="195" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="195" spans="3:9" outlineLevel="1">
       <c r="C195" s="9" t="s">
         <v>224</v>
       </c>
@@ -4423,7 +4439,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="196" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="196" spans="3:9" outlineLevel="1">
       <c r="C196" s="9" t="s">
         <v>225</v>
       </c>
@@ -4436,7 +4452,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="197" spans="3:9" hidden="1" outlineLevel="1">
+    <row r="197" spans="3:9" outlineLevel="1">
       <c r="C197" s="22"/>
       <c r="D197" s="38"/>
       <c r="E197" s="38"/>
@@ -4445,7 +4461,7 @@
       <c r="H197" s="38"/>
       <c r="I197" s="38"/>
     </row>
-    <row r="198" spans="3:9" collapsed="1">
+    <row r="198" spans="3:9">
       <c r="C198" s="20" t="s">
         <v>226</v>
       </c>
@@ -4651,7 +4667,7 @@
       <c r="H214" s="38"/>
       <c r="I214" s="38"/>
     </row>
-    <row r="215" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="215" spans="2:9" outlineLevel="1">
       <c r="C215" s="9" t="s">
         <v>243</v>
       </c>
@@ -4664,7 +4680,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="216" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="216" spans="2:9" outlineLevel="1">
       <c r="C216" s="9" t="s">
         <v>244</v>
       </c>
@@ -4677,7 +4693,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="217" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="217" spans="2:9" outlineLevel="1">
       <c r="C217" s="9" t="s">
         <v>245</v>
       </c>
@@ -4690,7 +4706,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="218" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="218" spans="2:9" outlineLevel="1">
       <c r="C218" s="9" t="s">
         <v>246</v>
       </c>
@@ -4703,7 +4719,7 @@
       </c>
       <c r="I218" s="21"/>
     </row>
-    <row r="219" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="219" spans="2:9" outlineLevel="1">
       <c r="C219" s="9" t="s">
         <v>248</v>
       </c>
@@ -4716,7 +4732,7 @@
       </c>
       <c r="I219" s="21"/>
     </row>
-    <row r="220" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="220" spans="2:9" outlineLevel="1">
       <c r="C220" s="9" t="s">
         <v>249</v>
       </c>
@@ -4729,7 +4745,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="221" spans="2:9" outlineLevel="1">
       <c r="C221" s="9" t="s">
         <v>251</v>
       </c>
@@ -4742,7 +4758,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="2:9" hidden="1" outlineLevel="1">
+    <row r="222" spans="2:9" outlineLevel="1">
       <c r="C222" s="22"/>
       <c r="D222" s="38"/>
       <c r="E222" s="38"/>
@@ -4751,7 +4767,7 @@
       <c r="H222" s="38"/>
       <c r="I222" s="38"/>
     </row>
-    <row r="223" spans="2:9" collapsed="1">
+    <row r="223" spans="2:9">
       <c r="C223" s="20" t="s">
         <v>252</v>
       </c>
@@ -5002,7 +5018,7 @@
       <c r="H244" s="21"/>
       <c r="I244" s="21"/>
     </row>
-    <row r="245" spans="3:9" outlineLevel="1">
+    <row r="245" spans="3:9" ht="28" outlineLevel="1">
       <c r="C245" s="11" t="s">
         <v>280</v>
       </c>
@@ -5109,7 +5125,7 @@
       </c>
       <c r="D254" s="32"/>
     </row>
-    <row r="255" spans="3:9" outlineLevel="1">
+    <row r="255" spans="3:9" ht="28" outlineLevel="1">
       <c r="C255" s="2" t="s">
         <v>292</v>
       </c>
@@ -5257,7 +5273,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="271" spans="3:9" outlineLevel="1">
+    <row r="271" spans="3:9" ht="28" outlineLevel="1">
       <c r="C271" s="14" t="s">
         <v>308</v>
       </c>
@@ -5654,7 +5670,7 @@
       </c>
       <c r="I307" s="21"/>
     </row>
-    <row r="308" spans="3:9" outlineLevel="1">
+    <row r="308" spans="3:9" ht="27" outlineLevel="1">
       <c r="C308" s="31" t="s">
         <v>356</v>
       </c>

</xml_diff>